<commit_message>
fix: TypeError: Cannot read property 'findCell' of undefined      at WorkSheetHelper.eachCell (.../app/worksheet-helper.js:72:34)
</commit_message>
<xml_diff>
--- a/test-data/xlsx-template-ex-2.xlsx
+++ b/test-data/xlsx-template-ex-2.xlsx
@@ -1,18 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MVP\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18990" windowHeight="4635" activeTab="2"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Лист1" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Лист2" sheetId="2" r:id="rId4"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t xml:space="preserve">ОТЧЕТ ОБ ИНСПЕКЦИИ </t>
   </si>
@@ -133,45 +142,51 @@
   <si>
     <t>Подпись</t>
   </si>
+  <si>
+    <t>с текстом пусть будет</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="16.0"/>
+      <sz val="16"/>
       <name val="Times New Roman"/>
     </font>
     <font>
-      <sz val="18.0"/>
+      <sz val="18"/>
       <name val="Times New Roman"/>
     </font>
-    <font/>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
     <font>
       <b/>
       <u/>
-      <sz val="16.0"/>
+      <sz val="16"/>
       <name val="Times New Roman"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <name val="Times New Roman"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <name val="Times New Roman"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -181,7 +196,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -191,11 +206,21 @@
     </fill>
   </fills>
   <borders count="14">
-    <border/>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -210,6 +235,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -224,6 +250,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -238,6 +265,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -252,6 +280,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -266,6 +295,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -280,6 +310,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -291,6 +322,8 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -305,6 +338,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -313,6 +347,9 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -321,135 +358,402 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="32">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="2" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="0" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="0" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="2" fillId="0" fontId="7" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="3" fillId="0" fontId="7" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="4" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="0" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="4" fillId="0" fontId="0" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="6" fillId="0" fontId="0" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+  <a:themeElements>
+    <a:clrScheme name="Стандартная">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Стандартная">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Стандартная">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="52.0"/>
-    <col customWidth="1" min="2" max="2" width="49.86"/>
-    <col customWidth="1" min="3" max="12" width="8.57"/>
-    <col customWidth="1" min="13" max="26" width="8.71"/>
+    <col min="1" max="1" width="52" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" customWidth="1"/>
+    <col min="3" max="12" width="8.5703125" customWidth="1"/>
+    <col min="13" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.75" customHeight="1">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -477,10 +781,11 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="23"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -506,11 +811,11 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" ht="21.75" customHeight="1">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="30"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -536,9 +841,9 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
+    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -564,10 +869,11 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
         <v>2</v>
       </c>
+      <c r="B5" s="23"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -593,9 +899,9 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" ht="9.75" customHeight="1">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
+    <row r="6" spans="1:26" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -621,11 +927,11 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" ht="18.0" customHeight="1">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1"/>
@@ -653,11 +959,11 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" ht="32.25" customHeight="1">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="1"/>
@@ -685,11 +991,11 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" ht="37.5" customHeight="1">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:26" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="1"/>
@@ -717,11 +1023,11 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" ht="48.75" customHeight="1">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:26" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="1"/>
@@ -749,11 +1055,11 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="1"/>
@@ -781,11 +1087,11 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
-    <row r="12" ht="30.0" customHeight="1">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="1"/>
@@ -813,11 +1119,11 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" ht="26.25" customHeight="1">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="1"/>
@@ -845,11 +1151,11 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" ht="30.75" customHeight="1">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:26" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="1"/>
@@ -877,11 +1183,11 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" ht="31.5" customHeight="1">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:26" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="1"/>
@@ -909,11 +1215,11 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" ht="29.25" customHeight="1">
-      <c r="A16" s="13" t="s">
+    <row r="16" spans="1:26" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="1"/>
@@ -941,8 +1247,9 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" ht="12.0" customHeight="1">
-      <c r="A17" s="6"/>
+    <row r="17" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="22"/>
+      <c r="B17" s="23"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -968,10 +1275,11 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="6" t="s">
+    <row r="18" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
         <v>23</v>
       </c>
+      <c r="B18" s="23"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -997,9 +1305,9 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" ht="10.5" customHeight="1">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
+    <row r="19" spans="1:26" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1025,23 +1333,23 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="7" t="s">
+    <row r="20" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="16"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="13"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
@@ -1057,23 +1365,23 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" s="13" t="s">
+    <row r="21" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="1"/>
-      <c r="D21" s="16"/>
+      <c r="D21" s="13"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="16"/>
+      <c r="F21" s="13"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="16"/>
+      <c r="H21" s="13"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="16"/>
+      <c r="J21" s="13"/>
       <c r="K21" s="1"/>
-      <c r="L21" s="16"/>
+      <c r="L21" s="13"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
@@ -1089,9 +1397,9 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
+    <row r="22" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1117,10 +1425,11 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" s="6" t="s">
+    <row r="23" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="22" t="s">
         <v>28</v>
       </c>
+      <c r="B23" s="23"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1146,7 +1455,7 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" ht="6.0" customHeight="1">
+    <row r="24" spans="1:26" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1174,11 +1483,11 @@
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
     </row>
-    <row r="25" ht="12.75" customHeight="1">
-      <c r="A25" s="17" t="s">
+    <row r="25" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="14" t="s">
         <v>30</v>
       </c>
       <c r="C25" s="1"/>
@@ -1206,9 +1515,9 @@
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
     </row>
-    <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" s="19"/>
-      <c r="B26" s="18" t="s">
+    <row r="26" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="27"/>
+      <c r="B26" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C26" s="1"/>
@@ -1236,9 +1545,9 @@
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
     </row>
-    <row r="27" ht="33.0" customHeight="1">
-      <c r="A27" s="20"/>
-      <c r="B27" s="18" t="s">
+    <row r="27" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="28"/>
+      <c r="B27" s="14" t="s">
         <v>32</v>
       </c>
       <c r="C27" s="1"/>
@@ -1266,7 +1575,7 @@
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
     </row>
-    <row r="28" ht="5.25" customHeight="1">
+    <row r="28" spans="1:26" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1294,10 +1603,11 @@
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
     </row>
-    <row r="29" ht="12.75" customHeight="1">
-      <c r="A29" s="6" t="s">
+    <row r="29" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
         <v>33</v>
       </c>
+      <c r="B29" s="23"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1323,7 +1633,7 @@
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
     </row>
-    <row r="30" ht="12.75" customHeight="1">
+    <row r="30" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1351,11 +1661,11 @@
       <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
     </row>
-    <row r="31" ht="12.75" customHeight="1">
-      <c r="A31" s="21" t="s">
+    <row r="31" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="22"/>
+      <c r="B31" s="25"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -1381,11 +1691,11 @@
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
     </row>
-    <row r="32" ht="147.0" customHeight="1">
-      <c r="A32" s="23" t="s">
+    <row r="32" spans="1:26" ht="147" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="24"/>
+      <c r="B32" s="15"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1411,11 +1721,11 @@
       <c r="Y32" s="1"/>
       <c r="Z32" s="1"/>
     </row>
-    <row r="33" ht="12.75" customHeight="1">
-      <c r="A33" s="23" t="s">
+    <row r="33" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="24"/>
+      <c r="B33" s="15"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -1441,7 +1751,7 @@
       <c r="Y33" s="1"/>
       <c r="Z33" s="1"/>
     </row>
-    <row r="34" ht="12.75" customHeight="1">
+    <row r="34" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1469,10 +1779,11 @@
       <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
     </row>
-    <row r="35" ht="12.75" customHeight="1">
-      <c r="A35" s="6" t="s">
+    <row r="35" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="22" t="s">
         <v>37</v>
       </c>
+      <c r="B35" s="23"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -1498,7 +1809,7 @@
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
     </row>
-    <row r="36" ht="12.75" customHeight="1">
+    <row r="36" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1526,11 +1837,11 @@
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
     </row>
-    <row r="37" ht="12.75" customHeight="1">
-      <c r="A37" s="25" t="s">
+    <row r="37" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="26" t="s">
+      <c r="B37" s="17" t="s">
         <v>39</v>
       </c>
       <c r="C37" s="1"/>
@@ -1558,11 +1869,11 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" ht="12.75" customHeight="1">
-      <c r="A38" s="27" t="s">
+    <row r="38" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="28"/>
+      <c r="B38" s="19"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -1588,9 +1899,9 @@
       <c r="Y38" s="1"/>
       <c r="Z38" s="1"/>
     </row>
-    <row r="39" ht="12.75" customHeight="1">
-      <c r="A39" s="29"/>
-      <c r="B39" s="28"/>
+    <row r="39" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="20"/>
+      <c r="B39" s="19"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -1616,9 +1927,9 @@
       <c r="Y39" s="1"/>
       <c r="Z39" s="1"/>
     </row>
-    <row r="40" ht="12.75" customHeight="1">
-      <c r="A40" s="29"/>
-      <c r="B40" s="28"/>
+    <row r="40" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="20"/>
+      <c r="B40" s="19"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -1644,9 +1955,9 @@
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
     </row>
-    <row r="41" ht="12.75" customHeight="1">
-      <c r="A41" s="29"/>
-      <c r="B41" s="28"/>
+    <row r="41" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="20"/>
+      <c r="B41" s="19"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -1672,9 +1983,9 @@
       <c r="Y41" s="1"/>
       <c r="Z41" s="1"/>
     </row>
-    <row r="42" ht="12.75" customHeight="1">
-      <c r="A42" s="29"/>
-      <c r="B42" s="28"/>
+    <row r="42" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="20"/>
+      <c r="B42" s="19"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -1700,9 +2011,9 @@
       <c r="Y42" s="1"/>
       <c r="Z42" s="1"/>
     </row>
-    <row r="43" ht="12.75" customHeight="1">
-      <c r="A43" s="30"/>
-      <c r="B43" s="28"/>
+    <row r="43" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="21"/>
+      <c r="B43" s="19"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -1728,7 +2039,7 @@
       <c r="Y43" s="1"/>
       <c r="Z43" s="1"/>
     </row>
-    <row r="44" ht="12.75" customHeight="1">
+    <row r="44" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1756,7 +2067,7 @@
       <c r="Y44" s="1"/>
       <c r="Z44" s="1"/>
     </row>
-    <row r="45" ht="12.75" customHeight="1">
+    <row r="45" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1784,7 +2095,7 @@
       <c r="Y45" s="1"/>
       <c r="Z45" s="1"/>
     </row>
-    <row r="46" ht="12.75" customHeight="1">
+    <row r="46" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1812,7 +2123,7 @@
       <c r="Y46" s="1"/>
       <c r="Z46" s="1"/>
     </row>
-    <row r="47" ht="12.75" customHeight="1">
+    <row r="47" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1840,7 +2151,7 @@
       <c r="Y47" s="1"/>
       <c r="Z47" s="1"/>
     </row>
-    <row r="48" ht="12.75" customHeight="1">
+    <row r="48" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1868,7 +2179,7 @@
       <c r="Y48" s="1"/>
       <c r="Z48" s="1"/>
     </row>
-    <row r="49" ht="12.75" customHeight="1">
+    <row r="49" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1896,7 +2207,7 @@
       <c r="Y49" s="1"/>
       <c r="Z49" s="1"/>
     </row>
-    <row r="50" ht="12.75" customHeight="1">
+    <row r="50" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1924,7 +2235,7 @@
       <c r="Y50" s="1"/>
       <c r="Z50" s="1"/>
     </row>
-    <row r="51" ht="12.75" customHeight="1">
+    <row r="51" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1952,7 +2263,7 @@
       <c r="Y51" s="1"/>
       <c r="Z51" s="1"/>
     </row>
-    <row r="52" ht="12.75" customHeight="1">
+    <row r="52" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1980,7 +2291,7 @@
       <c r="Y52" s="1"/>
       <c r="Z52" s="1"/>
     </row>
-    <row r="53" ht="12.75" customHeight="1">
+    <row r="53" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2008,7 +2319,7 @@
       <c r="Y53" s="1"/>
       <c r="Z53" s="1"/>
     </row>
-    <row r="54" ht="12.75" customHeight="1">
+    <row r="54" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2036,7 +2347,7 @@
       <c r="Y54" s="1"/>
       <c r="Z54" s="1"/>
     </row>
-    <row r="55" ht="12.75" customHeight="1">
+    <row r="55" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2064,7 +2375,7 @@
       <c r="Y55" s="1"/>
       <c r="Z55" s="1"/>
     </row>
-    <row r="56" ht="12.75" customHeight="1">
+    <row r="56" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2092,7 +2403,7 @@
       <c r="Y56" s="1"/>
       <c r="Z56" s="1"/>
     </row>
-    <row r="57" ht="12.75" customHeight="1">
+    <row r="57" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2120,7 +2431,7 @@
       <c r="Y57" s="1"/>
       <c r="Z57" s="1"/>
     </row>
-    <row r="58" ht="12.75" customHeight="1">
+    <row r="58" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2148,7 +2459,7 @@
       <c r="Y58" s="1"/>
       <c r="Z58" s="1"/>
     </row>
-    <row r="59" ht="12.75" customHeight="1">
+    <row r="59" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2176,7 +2487,7 @@
       <c r="Y59" s="1"/>
       <c r="Z59" s="1"/>
     </row>
-    <row r="60" ht="12.75" customHeight="1">
+    <row r="60" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2204,7 +2515,7 @@
       <c r="Y60" s="1"/>
       <c r="Z60" s="1"/>
     </row>
-    <row r="61" ht="12.75" customHeight="1">
+    <row r="61" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2232,7 +2543,7 @@
       <c r="Y61" s="1"/>
       <c r="Z61" s="1"/>
     </row>
-    <row r="62" ht="12.75" customHeight="1">
+    <row r="62" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2260,7 +2571,7 @@
       <c r="Y62" s="1"/>
       <c r="Z62" s="1"/>
     </row>
-    <row r="63" ht="12.75" customHeight="1">
+    <row r="63" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2288,7 +2599,7 @@
       <c r="Y63" s="1"/>
       <c r="Z63" s="1"/>
     </row>
-    <row r="64" ht="12.75" customHeight="1">
+    <row r="64" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2316,7 +2627,7 @@
       <c r="Y64" s="1"/>
       <c r="Z64" s="1"/>
     </row>
-    <row r="65" ht="12.75" customHeight="1">
+    <row r="65" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2344,7 +2655,7 @@
       <c r="Y65" s="1"/>
       <c r="Z65" s="1"/>
     </row>
-    <row r="66" ht="12.75" customHeight="1">
+    <row r="66" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2372,7 +2683,7 @@
       <c r="Y66" s="1"/>
       <c r="Z66" s="1"/>
     </row>
-    <row r="67" ht="12.75" customHeight="1">
+    <row r="67" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2400,7 +2711,7 @@
       <c r="Y67" s="1"/>
       <c r="Z67" s="1"/>
     </row>
-    <row r="68" ht="12.75" customHeight="1">
+    <row r="68" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2428,7 +2739,7 @@
       <c r="Y68" s="1"/>
       <c r="Z68" s="1"/>
     </row>
-    <row r="69" ht="12.75" customHeight="1">
+    <row r="69" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2456,7 +2767,7 @@
       <c r="Y69" s="1"/>
       <c r="Z69" s="1"/>
     </row>
-    <row r="70" ht="12.75" customHeight="1">
+    <row r="70" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2484,7 +2795,7 @@
       <c r="Y70" s="1"/>
       <c r="Z70" s="1"/>
     </row>
-    <row r="71" ht="12.75" customHeight="1">
+    <row r="71" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2512,7 +2823,7 @@
       <c r="Y71" s="1"/>
       <c r="Z71" s="1"/>
     </row>
-    <row r="72" ht="12.75" customHeight="1">
+    <row r="72" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2540,7 +2851,7 @@
       <c r="Y72" s="1"/>
       <c r="Z72" s="1"/>
     </row>
-    <row r="73" ht="12.75" customHeight="1">
+    <row r="73" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2568,7 +2879,7 @@
       <c r="Y73" s="1"/>
       <c r="Z73" s="1"/>
     </row>
-    <row r="74" ht="12.75" customHeight="1">
+    <row r="74" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2596,7 +2907,7 @@
       <c r="Y74" s="1"/>
       <c r="Z74" s="1"/>
     </row>
-    <row r="75" ht="12.75" customHeight="1">
+    <row r="75" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2624,7 +2935,7 @@
       <c r="Y75" s="1"/>
       <c r="Z75" s="1"/>
     </row>
-    <row r="76" ht="12.75" customHeight="1">
+    <row r="76" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2652,7 +2963,7 @@
       <c r="Y76" s="1"/>
       <c r="Z76" s="1"/>
     </row>
-    <row r="77" ht="12.75" customHeight="1">
+    <row r="77" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2680,7 +2991,7 @@
       <c r="Y77" s="1"/>
       <c r="Z77" s="1"/>
     </row>
-    <row r="78" ht="12.75" customHeight="1">
+    <row r="78" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2708,7 +3019,7 @@
       <c r="Y78" s="1"/>
       <c r="Z78" s="1"/>
     </row>
-    <row r="79" ht="12.75" customHeight="1">
+    <row r="79" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2736,7 +3047,7 @@
       <c r="Y79" s="1"/>
       <c r="Z79" s="1"/>
     </row>
-    <row r="80" ht="12.75" customHeight="1">
+    <row r="80" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2764,7 +3075,7 @@
       <c r="Y80" s="1"/>
       <c r="Z80" s="1"/>
     </row>
-    <row r="81" ht="12.75" customHeight="1">
+    <row r="81" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2792,7 +3103,7 @@
       <c r="Y81" s="1"/>
       <c r="Z81" s="1"/>
     </row>
-    <row r="82" ht="12.75" customHeight="1">
+    <row r="82" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2820,7 +3131,7 @@
       <c r="Y82" s="1"/>
       <c r="Z82" s="1"/>
     </row>
-    <row r="83" ht="12.75" customHeight="1">
+    <row r="83" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2848,7 +3159,7 @@
       <c r="Y83" s="1"/>
       <c r="Z83" s="1"/>
     </row>
-    <row r="84" ht="12.75" customHeight="1">
+    <row r="84" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2876,7 +3187,7 @@
       <c r="Y84" s="1"/>
       <c r="Z84" s="1"/>
     </row>
-    <row r="85" ht="12.75" customHeight="1">
+    <row r="85" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2904,7 +3215,7 @@
       <c r="Y85" s="1"/>
       <c r="Z85" s="1"/>
     </row>
-    <row r="86" ht="12.75" customHeight="1">
+    <row r="86" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2932,7 +3243,7 @@
       <c r="Y86" s="1"/>
       <c r="Z86" s="1"/>
     </row>
-    <row r="87" ht="12.75" customHeight="1">
+    <row r="87" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2960,7 +3271,7 @@
       <c r="Y87" s="1"/>
       <c r="Z87" s="1"/>
     </row>
-    <row r="88" ht="12.75" customHeight="1">
+    <row r="88" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2988,7 +3299,7 @@
       <c r="Y88" s="1"/>
       <c r="Z88" s="1"/>
     </row>
-    <row r="89" ht="12.75" customHeight="1">
+    <row r="89" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -3016,7 +3327,7 @@
       <c r="Y89" s="1"/>
       <c r="Z89" s="1"/>
     </row>
-    <row r="90" ht="12.75" customHeight="1">
+    <row r="90" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -3044,7 +3355,7 @@
       <c r="Y90" s="1"/>
       <c r="Z90" s="1"/>
     </row>
-    <row r="91" ht="12.75" customHeight="1">
+    <row r="91" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -3072,7 +3383,7 @@
       <c r="Y91" s="1"/>
       <c r="Z91" s="1"/>
     </row>
-    <row r="92" ht="12.75" customHeight="1">
+    <row r="92" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -3100,7 +3411,7 @@
       <c r="Y92" s="1"/>
       <c r="Z92" s="1"/>
     </row>
-    <row r="93" ht="12.75" customHeight="1">
+    <row r="93" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -3128,7 +3439,7 @@
       <c r="Y93" s="1"/>
       <c r="Z93" s="1"/>
     </row>
-    <row r="94" ht="12.75" customHeight="1">
+    <row r="94" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -3156,7 +3467,7 @@
       <c r="Y94" s="1"/>
       <c r="Z94" s="1"/>
     </row>
-    <row r="95" ht="12.75" customHeight="1">
+    <row r="95" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -3184,7 +3495,7 @@
       <c r="Y95" s="1"/>
       <c r="Z95" s="1"/>
     </row>
-    <row r="96" ht="12.75" customHeight="1">
+    <row r="96" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -3212,7 +3523,7 @@
       <c r="Y96" s="1"/>
       <c r="Z96" s="1"/>
     </row>
-    <row r="97" ht="12.75" customHeight="1">
+    <row r="97" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -3240,7 +3551,7 @@
       <c r="Y97" s="1"/>
       <c r="Z97" s="1"/>
     </row>
-    <row r="98" ht="12.75" customHeight="1">
+    <row r="98" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -3268,7 +3579,7 @@
       <c r="Y98" s="1"/>
       <c r="Z98" s="1"/>
     </row>
-    <row r="99" ht="12.75" customHeight="1">
+    <row r="99" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -3296,7 +3607,7 @@
       <c r="Y99" s="1"/>
       <c r="Z99" s="1"/>
     </row>
-    <row r="100" ht="12.75" customHeight="1">
+    <row r="100" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -3324,7 +3635,7 @@
       <c r="Y100" s="1"/>
       <c r="Z100" s="1"/>
     </row>
-    <row r="101" ht="12.75" customHeight="1">
+    <row r="101" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -3352,7 +3663,7 @@
       <c r="Y101" s="1"/>
       <c r="Z101" s="1"/>
     </row>
-    <row r="102" ht="12.75" customHeight="1">
+    <row r="102" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -3380,7 +3691,7 @@
       <c r="Y102" s="1"/>
       <c r="Z102" s="1"/>
     </row>
-    <row r="103" ht="12.75" customHeight="1">
+    <row r="103" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -3408,7 +3719,7 @@
       <c r="Y103" s="1"/>
       <c r="Z103" s="1"/>
     </row>
-    <row r="104" ht="12.75" customHeight="1">
+    <row r="104" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -3436,7 +3747,7 @@
       <c r="Y104" s="1"/>
       <c r="Z104" s="1"/>
     </row>
-    <row r="105" ht="12.75" customHeight="1">
+    <row r="105" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -3464,7 +3775,7 @@
       <c r="Y105" s="1"/>
       <c r="Z105" s="1"/>
     </row>
-    <row r="106" ht="12.75" customHeight="1">
+    <row r="106" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -3492,7 +3803,7 @@
       <c r="Y106" s="1"/>
       <c r="Z106" s="1"/>
     </row>
-    <row r="107" ht="12.75" customHeight="1">
+    <row r="107" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -3520,7 +3831,7 @@
       <c r="Y107" s="1"/>
       <c r="Z107" s="1"/>
     </row>
-    <row r="108" ht="12.75" customHeight="1">
+    <row r="108" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -3548,7 +3859,7 @@
       <c r="Y108" s="1"/>
       <c r="Z108" s="1"/>
     </row>
-    <row r="109" ht="12.75" customHeight="1">
+    <row r="109" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -3576,7 +3887,7 @@
       <c r="Y109" s="1"/>
       <c r="Z109" s="1"/>
     </row>
-    <row r="110" ht="12.75" customHeight="1">
+    <row r="110" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -3604,7 +3915,7 @@
       <c r="Y110" s="1"/>
       <c r="Z110" s="1"/>
     </row>
-    <row r="111" ht="12.75" customHeight="1">
+    <row r="111" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -3632,7 +3943,7 @@
       <c r="Y111" s="1"/>
       <c r="Z111" s="1"/>
     </row>
-    <row r="112" ht="12.75" customHeight="1">
+    <row r="112" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -3660,7 +3971,7 @@
       <c r="Y112" s="1"/>
       <c r="Z112" s="1"/>
     </row>
-    <row r="113" ht="12.75" customHeight="1">
+    <row r="113" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -3688,7 +3999,7 @@
       <c r="Y113" s="1"/>
       <c r="Z113" s="1"/>
     </row>
-    <row r="114" ht="12.75" customHeight="1">
+    <row r="114" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -3716,7 +4027,7 @@
       <c r="Y114" s="1"/>
       <c r="Z114" s="1"/>
     </row>
-    <row r="115" ht="12.75" customHeight="1">
+    <row r="115" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -3744,7 +4055,7 @@
       <c r="Y115" s="1"/>
       <c r="Z115" s="1"/>
     </row>
-    <row r="116" ht="12.75" customHeight="1">
+    <row r="116" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -3772,7 +4083,7 @@
       <c r="Y116" s="1"/>
       <c r="Z116" s="1"/>
     </row>
-    <row r="117" ht="12.75" customHeight="1">
+    <row r="117" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -3800,7 +4111,7 @@
       <c r="Y117" s="1"/>
       <c r="Z117" s="1"/>
     </row>
-    <row r="118" ht="12.75" customHeight="1">
+    <row r="118" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -3828,7 +4139,7 @@
       <c r="Y118" s="1"/>
       <c r="Z118" s="1"/>
     </row>
-    <row r="119" ht="12.75" customHeight="1">
+    <row r="119" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -3856,7 +4167,7 @@
       <c r="Y119" s="1"/>
       <c r="Z119" s="1"/>
     </row>
-    <row r="120" ht="12.75" customHeight="1">
+    <row r="120" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -3884,7 +4195,7 @@
       <c r="Y120" s="1"/>
       <c r="Z120" s="1"/>
     </row>
-    <row r="121" ht="12.75" customHeight="1">
+    <row r="121" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -3912,7 +4223,7 @@
       <c r="Y121" s="1"/>
       <c r="Z121" s="1"/>
     </row>
-    <row r="122" ht="12.75" customHeight="1">
+    <row r="122" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -3940,7 +4251,7 @@
       <c r="Y122" s="1"/>
       <c r="Z122" s="1"/>
     </row>
-    <row r="123" ht="12.75" customHeight="1">
+    <row r="123" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -3968,7 +4279,7 @@
       <c r="Y123" s="1"/>
       <c r="Z123" s="1"/>
     </row>
-    <row r="124" ht="12.75" customHeight="1">
+    <row r="124" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -3996,7 +4307,7 @@
       <c r="Y124" s="1"/>
       <c r="Z124" s="1"/>
     </row>
-    <row r="125" ht="12.75" customHeight="1">
+    <row r="125" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -4024,7 +4335,7 @@
       <c r="Y125" s="1"/>
       <c r="Z125" s="1"/>
     </row>
-    <row r="126" ht="12.75" customHeight="1">
+    <row r="126" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -4052,7 +4363,7 @@
       <c r="Y126" s="1"/>
       <c r="Z126" s="1"/>
     </row>
-    <row r="127" ht="12.75" customHeight="1">
+    <row r="127" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -4080,7 +4391,7 @@
       <c r="Y127" s="1"/>
       <c r="Z127" s="1"/>
     </row>
-    <row r="128" ht="12.75" customHeight="1">
+    <row r="128" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -4108,7 +4419,7 @@
       <c r="Y128" s="1"/>
       <c r="Z128" s="1"/>
     </row>
-    <row r="129" ht="12.75" customHeight="1">
+    <row r="129" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -4136,7 +4447,7 @@
       <c r="Y129" s="1"/>
       <c r="Z129" s="1"/>
     </row>
-    <row r="130" ht="12.75" customHeight="1">
+    <row r="130" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -4164,7 +4475,7 @@
       <c r="Y130" s="1"/>
       <c r="Z130" s="1"/>
     </row>
-    <row r="131" ht="12.75" customHeight="1">
+    <row r="131" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -4192,7 +4503,7 @@
       <c r="Y131" s="1"/>
       <c r="Z131" s="1"/>
     </row>
-    <row r="132" ht="12.75" customHeight="1">
+    <row r="132" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -4220,7 +4531,7 @@
       <c r="Y132" s="1"/>
       <c r="Z132" s="1"/>
     </row>
-    <row r="133" ht="12.75" customHeight="1">
+    <row r="133" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -4248,7 +4559,7 @@
       <c r="Y133" s="1"/>
       <c r="Z133" s="1"/>
     </row>
-    <row r="134" ht="12.75" customHeight="1">
+    <row r="134" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -4276,7 +4587,7 @@
       <c r="Y134" s="1"/>
       <c r="Z134" s="1"/>
     </row>
-    <row r="135" ht="12.75" customHeight="1">
+    <row r="135" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -4304,7 +4615,7 @@
       <c r="Y135" s="1"/>
       <c r="Z135" s="1"/>
     </row>
-    <row r="136" ht="12.75" customHeight="1">
+    <row r="136" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -4332,7 +4643,7 @@
       <c r="Y136" s="1"/>
       <c r="Z136" s="1"/>
     </row>
-    <row r="137" ht="12.75" customHeight="1">
+    <row r="137" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -4360,7 +4671,7 @@
       <c r="Y137" s="1"/>
       <c r="Z137" s="1"/>
     </row>
-    <row r="138" ht="12.75" customHeight="1">
+    <row r="138" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -4388,7 +4699,7 @@
       <c r="Y138" s="1"/>
       <c r="Z138" s="1"/>
     </row>
-    <row r="139" ht="12.75" customHeight="1">
+    <row r="139" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -4416,7 +4727,7 @@
       <c r="Y139" s="1"/>
       <c r="Z139" s="1"/>
     </row>
-    <row r="140" ht="12.75" customHeight="1">
+    <row r="140" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -4444,7 +4755,7 @@
       <c r="Y140" s="1"/>
       <c r="Z140" s="1"/>
     </row>
-    <row r="141" ht="12.75" customHeight="1">
+    <row r="141" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -4472,7 +4783,7 @@
       <c r="Y141" s="1"/>
       <c r="Z141" s="1"/>
     </row>
-    <row r="142" ht="12.75" customHeight="1">
+    <row r="142" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -4500,7 +4811,7 @@
       <c r="Y142" s="1"/>
       <c r="Z142" s="1"/>
     </row>
-    <row r="143" ht="12.75" customHeight="1">
+    <row r="143" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -4528,7 +4839,7 @@
       <c r="Y143" s="1"/>
       <c r="Z143" s="1"/>
     </row>
-    <row r="144" ht="12.75" customHeight="1">
+    <row r="144" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -4556,7 +4867,7 @@
       <c r="Y144" s="1"/>
       <c r="Z144" s="1"/>
     </row>
-    <row r="145" ht="12.75" customHeight="1">
+    <row r="145" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -4584,7 +4895,7 @@
       <c r="Y145" s="1"/>
       <c r="Z145" s="1"/>
     </row>
-    <row r="146" ht="12.75" customHeight="1">
+    <row r="146" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -4612,7 +4923,7 @@
       <c r="Y146" s="1"/>
       <c r="Z146" s="1"/>
     </row>
-    <row r="147" ht="12.75" customHeight="1">
+    <row r="147" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -4640,7 +4951,7 @@
       <c r="Y147" s="1"/>
       <c r="Z147" s="1"/>
     </row>
-    <row r="148" ht="12.75" customHeight="1">
+    <row r="148" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -4668,7 +4979,7 @@
       <c r="Y148" s="1"/>
       <c r="Z148" s="1"/>
     </row>
-    <row r="149" ht="12.75" customHeight="1">
+    <row r="149" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -4696,7 +5007,7 @@
       <c r="Y149" s="1"/>
       <c r="Z149" s="1"/>
     </row>
-    <row r="150" ht="12.75" customHeight="1">
+    <row r="150" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -4724,7 +5035,7 @@
       <c r="Y150" s="1"/>
       <c r="Z150" s="1"/>
     </row>
-    <row r="151" ht="12.75" customHeight="1">
+    <row r="151" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -4752,7 +5063,7 @@
       <c r="Y151" s="1"/>
       <c r="Z151" s="1"/>
     </row>
-    <row r="152" ht="12.75" customHeight="1">
+    <row r="152" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -4780,7 +5091,7 @@
       <c r="Y152" s="1"/>
       <c r="Z152" s="1"/>
     </row>
-    <row r="153" ht="12.75" customHeight="1">
+    <row r="153" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -4808,7 +5119,7 @@
       <c r="Y153" s="1"/>
       <c r="Z153" s="1"/>
     </row>
-    <row r="154" ht="12.75" customHeight="1">
+    <row r="154" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -4836,7 +5147,7 @@
       <c r="Y154" s="1"/>
       <c r="Z154" s="1"/>
     </row>
-    <row r="155" ht="12.75" customHeight="1">
+    <row r="155" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -4864,7 +5175,7 @@
       <c r="Y155" s="1"/>
       <c r="Z155" s="1"/>
     </row>
-    <row r="156" ht="12.75" customHeight="1">
+    <row r="156" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -4892,7 +5203,7 @@
       <c r="Y156" s="1"/>
       <c r="Z156" s="1"/>
     </row>
-    <row r="157" ht="12.75" customHeight="1">
+    <row r="157" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -4920,7 +5231,7 @@
       <c r="Y157" s="1"/>
       <c r="Z157" s="1"/>
     </row>
-    <row r="158" ht="12.75" customHeight="1">
+    <row r="158" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -4948,7 +5259,7 @@
       <c r="Y158" s="1"/>
       <c r="Z158" s="1"/>
     </row>
-    <row r="159" ht="12.75" customHeight="1">
+    <row r="159" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -4976,7 +5287,7 @@
       <c r="Y159" s="1"/>
       <c r="Z159" s="1"/>
     </row>
-    <row r="160" ht="12.75" customHeight="1">
+    <row r="160" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -5004,7 +5315,7 @@
       <c r="Y160" s="1"/>
       <c r="Z160" s="1"/>
     </row>
-    <row r="161" ht="12.75" customHeight="1">
+    <row r="161" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -5032,7 +5343,7 @@
       <c r="Y161" s="1"/>
       <c r="Z161" s="1"/>
     </row>
-    <row r="162" ht="12.75" customHeight="1">
+    <row r="162" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -5060,7 +5371,7 @@
       <c r="Y162" s="1"/>
       <c r="Z162" s="1"/>
     </row>
-    <row r="163" ht="12.75" customHeight="1">
+    <row r="163" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -5088,7 +5399,7 @@
       <c r="Y163" s="1"/>
       <c r="Z163" s="1"/>
     </row>
-    <row r="164" ht="12.75" customHeight="1">
+    <row r="164" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -5116,7 +5427,7 @@
       <c r="Y164" s="1"/>
       <c r="Z164" s="1"/>
     </row>
-    <row r="165" ht="12.75" customHeight="1">
+    <row r="165" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -5144,7 +5455,7 @@
       <c r="Y165" s="1"/>
       <c r="Z165" s="1"/>
     </row>
-    <row r="166" ht="12.75" customHeight="1">
+    <row r="166" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -5172,7 +5483,7 @@
       <c r="Y166" s="1"/>
       <c r="Z166" s="1"/>
     </row>
-    <row r="167" ht="12.75" customHeight="1">
+    <row r="167" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -5200,7 +5511,7 @@
       <c r="Y167" s="1"/>
       <c r="Z167" s="1"/>
     </row>
-    <row r="168" ht="12.75" customHeight="1">
+    <row r="168" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -5228,7 +5539,7 @@
       <c r="Y168" s="1"/>
       <c r="Z168" s="1"/>
     </row>
-    <row r="169" ht="12.75" customHeight="1">
+    <row r="169" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -5256,7 +5567,7 @@
       <c r="Y169" s="1"/>
       <c r="Z169" s="1"/>
     </row>
-    <row r="170" ht="12.75" customHeight="1">
+    <row r="170" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -5284,7 +5595,7 @@
       <c r="Y170" s="1"/>
       <c r="Z170" s="1"/>
     </row>
-    <row r="171" ht="12.75" customHeight="1">
+    <row r="171" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -5312,7 +5623,7 @@
       <c r="Y171" s="1"/>
       <c r="Z171" s="1"/>
     </row>
-    <row r="172" ht="12.75" customHeight="1">
+    <row r="172" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -5340,7 +5651,7 @@
       <c r="Y172" s="1"/>
       <c r="Z172" s="1"/>
     </row>
-    <row r="173" ht="12.75" customHeight="1">
+    <row r="173" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -5368,7 +5679,7 @@
       <c r="Y173" s="1"/>
       <c r="Z173" s="1"/>
     </row>
-    <row r="174" ht="12.75" customHeight="1">
+    <row r="174" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -5396,7 +5707,7 @@
       <c r="Y174" s="1"/>
       <c r="Z174" s="1"/>
     </row>
-    <row r="175" ht="12.75" customHeight="1">
+    <row r="175" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -5424,7 +5735,7 @@
       <c r="Y175" s="1"/>
       <c r="Z175" s="1"/>
     </row>
-    <row r="176" ht="12.75" customHeight="1">
+    <row r="176" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -5452,7 +5763,7 @@
       <c r="Y176" s="1"/>
       <c r="Z176" s="1"/>
     </row>
-    <row r="177" ht="12.75" customHeight="1">
+    <row r="177" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -5480,7 +5791,7 @@
       <c r="Y177" s="1"/>
       <c r="Z177" s="1"/>
     </row>
-    <row r="178" ht="12.75" customHeight="1">
+    <row r="178" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -5508,7 +5819,7 @@
       <c r="Y178" s="1"/>
       <c r="Z178" s="1"/>
     </row>
-    <row r="179" ht="12.75" customHeight="1">
+    <row r="179" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -5536,7 +5847,7 @@
       <c r="Y179" s="1"/>
       <c r="Z179" s="1"/>
     </row>
-    <row r="180" ht="12.75" customHeight="1">
+    <row r="180" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -5564,7 +5875,7 @@
       <c r="Y180" s="1"/>
       <c r="Z180" s="1"/>
     </row>
-    <row r="181" ht="12.75" customHeight="1">
+    <row r="181" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -5592,7 +5903,7 @@
       <c r="Y181" s="1"/>
       <c r="Z181" s="1"/>
     </row>
-    <row r="182" ht="12.75" customHeight="1">
+    <row r="182" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -5620,7 +5931,7 @@
       <c r="Y182" s="1"/>
       <c r="Z182" s="1"/>
     </row>
-    <row r="183" ht="12.75" customHeight="1">
+    <row r="183" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -5648,7 +5959,7 @@
       <c r="Y183" s="1"/>
       <c r="Z183" s="1"/>
     </row>
-    <row r="184" ht="12.75" customHeight="1">
+    <row r="184" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -5676,7 +5987,7 @@
       <c r="Y184" s="1"/>
       <c r="Z184" s="1"/>
     </row>
-    <row r="185" ht="12.75" customHeight="1">
+    <row r="185" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -5704,7 +6015,7 @@
       <c r="Y185" s="1"/>
       <c r="Z185" s="1"/>
     </row>
-    <row r="186" ht="12.75" customHeight="1">
+    <row r="186" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -5732,7 +6043,7 @@
       <c r="Y186" s="1"/>
       <c r="Z186" s="1"/>
     </row>
-    <row r="187" ht="12.75" customHeight="1">
+    <row r="187" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -5760,7 +6071,7 @@
       <c r="Y187" s="1"/>
       <c r="Z187" s="1"/>
     </row>
-    <row r="188" ht="12.75" customHeight="1">
+    <row r="188" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -5788,7 +6099,7 @@
       <c r="Y188" s="1"/>
       <c r="Z188" s="1"/>
     </row>
-    <row r="189" ht="12.75" customHeight="1">
+    <row r="189" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -5816,7 +6127,7 @@
       <c r="Y189" s="1"/>
       <c r="Z189" s="1"/>
     </row>
-    <row r="190" ht="12.75" customHeight="1">
+    <row r="190" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -5844,7 +6155,7 @@
       <c r="Y190" s="1"/>
       <c r="Z190" s="1"/>
     </row>
-    <row r="191" ht="12.75" customHeight="1">
+    <row r="191" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -5872,7 +6183,7 @@
       <c r="Y191" s="1"/>
       <c r="Z191" s="1"/>
     </row>
-    <row r="192" ht="12.75" customHeight="1">
+    <row r="192" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -5900,7 +6211,7 @@
       <c r="Y192" s="1"/>
       <c r="Z192" s="1"/>
     </row>
-    <row r="193" ht="12.75" customHeight="1">
+    <row r="193" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -5928,7 +6239,7 @@
       <c r="Y193" s="1"/>
       <c r="Z193" s="1"/>
     </row>
-    <row r="194" ht="12.75" customHeight="1">
+    <row r="194" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -5956,7 +6267,7 @@
       <c r="Y194" s="1"/>
       <c r="Z194" s="1"/>
     </row>
-    <row r="195" ht="12.75" customHeight="1">
+    <row r="195" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -5984,7 +6295,7 @@
       <c r="Y195" s="1"/>
       <c r="Z195" s="1"/>
     </row>
-    <row r="196" ht="12.75" customHeight="1">
+    <row r="196" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -6012,7 +6323,7 @@
       <c r="Y196" s="1"/>
       <c r="Z196" s="1"/>
     </row>
-    <row r="197" ht="12.75" customHeight="1">
+    <row r="197" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -6040,7 +6351,7 @@
       <c r="Y197" s="1"/>
       <c r="Z197" s="1"/>
     </row>
-    <row r="198" ht="12.75" customHeight="1">
+    <row r="198" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -6068,7 +6379,7 @@
       <c r="Y198" s="1"/>
       <c r="Z198" s="1"/>
     </row>
-    <row r="199" ht="12.75" customHeight="1">
+    <row r="199" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -6096,7 +6407,7 @@
       <c r="Y199" s="1"/>
       <c r="Z199" s="1"/>
     </row>
-    <row r="200" ht="12.75" customHeight="1">
+    <row r="200" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
@@ -6124,7 +6435,7 @@
       <c r="Y200" s="1"/>
       <c r="Z200" s="1"/>
     </row>
-    <row r="201" ht="12.75" customHeight="1">
+    <row r="201" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
@@ -6152,7 +6463,7 @@
       <c r="Y201" s="1"/>
       <c r="Z201" s="1"/>
     </row>
-    <row r="202" ht="12.75" customHeight="1">
+    <row r="202" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
@@ -6180,7 +6491,7 @@
       <c r="Y202" s="1"/>
       <c r="Z202" s="1"/>
     </row>
-    <row r="203" ht="12.75" customHeight="1">
+    <row r="203" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
@@ -6208,7 +6519,7 @@
       <c r="Y203" s="1"/>
       <c r="Z203" s="1"/>
     </row>
-    <row r="204" ht="12.75" customHeight="1">
+    <row r="204" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
@@ -6236,7 +6547,7 @@
       <c r="Y204" s="1"/>
       <c r="Z204" s="1"/>
     </row>
-    <row r="205" ht="12.75" customHeight="1">
+    <row r="205" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
@@ -6264,7 +6575,7 @@
       <c r="Y205" s="1"/>
       <c r="Z205" s="1"/>
     </row>
-    <row r="206" ht="12.75" customHeight="1">
+    <row r="206" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="1"/>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
@@ -6292,7 +6603,7 @@
       <c r="Y206" s="1"/>
       <c r="Z206" s="1"/>
     </row>
-    <row r="207" ht="12.75" customHeight="1">
+    <row r="207" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="1"/>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
@@ -6320,7 +6631,7 @@
       <c r="Y207" s="1"/>
       <c r="Z207" s="1"/>
     </row>
-    <row r="208" ht="12.75" customHeight="1">
+    <row r="208" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="1"/>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
@@ -6348,7 +6659,7 @@
       <c r="Y208" s="1"/>
       <c r="Z208" s="1"/>
     </row>
-    <row r="209" ht="12.75" customHeight="1">
+    <row r="209" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="1"/>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
@@ -6376,7 +6687,7 @@
       <c r="Y209" s="1"/>
       <c r="Z209" s="1"/>
     </row>
-    <row r="210" ht="12.75" customHeight="1">
+    <row r="210" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="1"/>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
@@ -6404,7 +6715,7 @@
       <c r="Y210" s="1"/>
       <c r="Z210" s="1"/>
     </row>
-    <row r="211" ht="12.75" customHeight="1">
+    <row r="211" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="1"/>
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
@@ -6432,7 +6743,7 @@
       <c r="Y211" s="1"/>
       <c r="Z211" s="1"/>
     </row>
-    <row r="212" ht="12.75" customHeight="1">
+    <row r="212" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="1"/>
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
@@ -6460,7 +6771,7 @@
       <c r="Y212" s="1"/>
       <c r="Z212" s="1"/>
     </row>
-    <row r="213" ht="12.75" customHeight="1">
+    <row r="213" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="1"/>
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
@@ -6488,7 +6799,7 @@
       <c r="Y213" s="1"/>
       <c r="Z213" s="1"/>
     </row>
-    <row r="214" ht="12.75" customHeight="1">
+    <row r="214" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="1"/>
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
@@ -6516,7 +6827,7 @@
       <c r="Y214" s="1"/>
       <c r="Z214" s="1"/>
     </row>
-    <row r="215" ht="12.75" customHeight="1">
+    <row r="215" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="1"/>
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
@@ -6544,7 +6855,7 @@
       <c r="Y215" s="1"/>
       <c r="Z215" s="1"/>
     </row>
-    <row r="216" ht="12.75" customHeight="1">
+    <row r="216" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="1"/>
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
@@ -6572,7 +6883,7 @@
       <c r="Y216" s="1"/>
       <c r="Z216" s="1"/>
     </row>
-    <row r="217" ht="12.75" customHeight="1">
+    <row r="217" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="1"/>
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
@@ -6600,7 +6911,7 @@
       <c r="Y217" s="1"/>
       <c r="Z217" s="1"/>
     </row>
-    <row r="218" ht="12.75" customHeight="1">
+    <row r="218" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="1"/>
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
@@ -6628,7 +6939,7 @@
       <c r="Y218" s="1"/>
       <c r="Z218" s="1"/>
     </row>
-    <row r="219" ht="12.75" customHeight="1">
+    <row r="219" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="1"/>
       <c r="B219" s="1"/>
       <c r="C219" s="1"/>
@@ -6656,7 +6967,7 @@
       <c r="Y219" s="1"/>
       <c r="Z219" s="1"/>
     </row>
-    <row r="220" ht="12.75" customHeight="1">
+    <row r="220" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="1"/>
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
@@ -6684,7 +6995,7 @@
       <c r="Y220" s="1"/>
       <c r="Z220" s="1"/>
     </row>
-    <row r="221" ht="12.75" customHeight="1">
+    <row r="221" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="1"/>
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
@@ -6712,7 +7023,7 @@
       <c r="Y221" s="1"/>
       <c r="Z221" s="1"/>
     </row>
-    <row r="222" ht="12.75" customHeight="1">
+    <row r="222" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="1"/>
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
@@ -6740,7 +7051,7 @@
       <c r="Y222" s="1"/>
       <c r="Z222" s="1"/>
     </row>
-    <row r="223" ht="12.75" customHeight="1">
+    <row r="223" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1"/>
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
@@ -6768,7 +7079,7 @@
       <c r="Y223" s="1"/>
       <c r="Z223" s="1"/>
     </row>
-    <row r="224" ht="12.75" customHeight="1">
+    <row r="224" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="1"/>
       <c r="B224" s="1"/>
       <c r="C224" s="1"/>
@@ -6796,7 +7107,7 @@
       <c r="Y224" s="1"/>
       <c r="Z224" s="1"/>
     </row>
-    <row r="225" ht="12.75" customHeight="1">
+    <row r="225" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="1"/>
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
@@ -6824,7 +7135,7 @@
       <c r="Y225" s="1"/>
       <c r="Z225" s="1"/>
     </row>
-    <row r="226" ht="12.75" customHeight="1">
+    <row r="226" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="1"/>
       <c r="B226" s="1"/>
       <c r="C226" s="1"/>
@@ -6852,7 +7163,7 @@
       <c r="Y226" s="1"/>
       <c r="Z226" s="1"/>
     </row>
-    <row r="227" ht="12.75" customHeight="1">
+    <row r="227" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="1"/>
       <c r="B227" s="1"/>
       <c r="C227" s="1"/>
@@ -6880,7 +7191,7 @@
       <c r="Y227" s="1"/>
       <c r="Z227" s="1"/>
     </row>
-    <row r="228" ht="12.75" customHeight="1">
+    <row r="228" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="1"/>
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
@@ -6908,7 +7219,7 @@
       <c r="Y228" s="1"/>
       <c r="Z228" s="1"/>
     </row>
-    <row r="229" ht="12.75" customHeight="1">
+    <row r="229" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="1"/>
       <c r="B229" s="1"/>
       <c r="C229" s="1"/>
@@ -6936,7 +7247,7 @@
       <c r="Y229" s="1"/>
       <c r="Z229" s="1"/>
     </row>
-    <row r="230" ht="12.75" customHeight="1">
+    <row r="230" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="1"/>
       <c r="B230" s="1"/>
       <c r="C230" s="1"/>
@@ -6964,7 +7275,7 @@
       <c r="Y230" s="1"/>
       <c r="Z230" s="1"/>
     </row>
-    <row r="231" ht="12.75" customHeight="1">
+    <row r="231" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="1"/>
       <c r="B231" s="1"/>
       <c r="C231" s="1"/>
@@ -6992,7 +7303,7 @@
       <c r="Y231" s="1"/>
       <c r="Z231" s="1"/>
     </row>
-    <row r="232" ht="12.75" customHeight="1">
+    <row r="232" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="1"/>
       <c r="B232" s="1"/>
       <c r="C232" s="1"/>
@@ -7020,7 +7331,7 @@
       <c r="Y232" s="1"/>
       <c r="Z232" s="1"/>
     </row>
-    <row r="233" ht="12.75" customHeight="1">
+    <row r="233" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="1"/>
       <c r="B233" s="1"/>
       <c r="C233" s="1"/>
@@ -7048,7 +7359,7 @@
       <c r="Y233" s="1"/>
       <c r="Z233" s="1"/>
     </row>
-    <row r="234" ht="12.75" customHeight="1">
+    <row r="234" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="1"/>
       <c r="B234" s="1"/>
       <c r="C234" s="1"/>
@@ -7076,7 +7387,7 @@
       <c r="Y234" s="1"/>
       <c r="Z234" s="1"/>
     </row>
-    <row r="235" ht="12.75" customHeight="1">
+    <row r="235" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="1"/>
       <c r="B235" s="1"/>
       <c r="C235" s="1"/>
@@ -7104,7 +7415,7 @@
       <c r="Y235" s="1"/>
       <c r="Z235" s="1"/>
     </row>
-    <row r="236" ht="12.75" customHeight="1">
+    <row r="236" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="1"/>
       <c r="B236" s="1"/>
       <c r="C236" s="1"/>
@@ -7132,7 +7443,7 @@
       <c r="Y236" s="1"/>
       <c r="Z236" s="1"/>
     </row>
-    <row r="237" ht="12.75" customHeight="1">
+    <row r="237" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="1"/>
       <c r="B237" s="1"/>
       <c r="C237" s="1"/>
@@ -7160,769 +7471,769 @@
       <c r="Y237" s="1"/>
       <c r="Z237" s="1"/>
     </row>
-    <row r="238" ht="15.75" customHeight="1"/>
-    <row r="239" ht="15.75" customHeight="1"/>
-    <row r="240" ht="15.75" customHeight="1"/>
-    <row r="241" ht="15.75" customHeight="1"/>
-    <row r="242" ht="15.75" customHeight="1"/>
-    <row r="243" ht="15.75" customHeight="1"/>
-    <row r="244" ht="15.75" customHeight="1"/>
-    <row r="245" ht="15.75" customHeight="1"/>
-    <row r="246" ht="15.75" customHeight="1"/>
-    <row r="247" ht="15.75" customHeight="1"/>
-    <row r="248" ht="15.75" customHeight="1"/>
-    <row r="249" ht="15.75" customHeight="1"/>
-    <row r="250" ht="15.75" customHeight="1"/>
-    <row r="251" ht="15.75" customHeight="1"/>
-    <row r="252" ht="15.75" customHeight="1"/>
-    <row r="253" ht="15.75" customHeight="1"/>
-    <row r="254" ht="15.75" customHeight="1"/>
-    <row r="255" ht="15.75" customHeight="1"/>
-    <row r="256" ht="15.75" customHeight="1"/>
-    <row r="257" ht="15.75" customHeight="1"/>
-    <row r="258" ht="15.75" customHeight="1"/>
-    <row r="259" ht="15.75" customHeight="1"/>
-    <row r="260" ht="15.75" customHeight="1"/>
-    <row r="261" ht="15.75" customHeight="1"/>
-    <row r="262" ht="15.75" customHeight="1"/>
-    <row r="263" ht="15.75" customHeight="1"/>
-    <row r="264" ht="15.75" customHeight="1"/>
-    <row r="265" ht="15.75" customHeight="1"/>
-    <row r="266" ht="15.75" customHeight="1"/>
-    <row r="267" ht="15.75" customHeight="1"/>
-    <row r="268" ht="15.75" customHeight="1"/>
-    <row r="269" ht="15.75" customHeight="1"/>
-    <row r="270" ht="15.75" customHeight="1"/>
-    <row r="271" ht="15.75" customHeight="1"/>
-    <row r="272" ht="15.75" customHeight="1"/>
-    <row r="273" ht="15.75" customHeight="1"/>
-    <row r="274" ht="15.75" customHeight="1"/>
-    <row r="275" ht="15.75" customHeight="1"/>
-    <row r="276" ht="15.75" customHeight="1"/>
-    <row r="277" ht="15.75" customHeight="1"/>
-    <row r="278" ht="15.75" customHeight="1"/>
-    <row r="279" ht="15.75" customHeight="1"/>
-    <row r="280" ht="15.75" customHeight="1"/>
-    <row r="281" ht="15.75" customHeight="1"/>
-    <row r="282" ht="15.75" customHeight="1"/>
-    <row r="283" ht="15.75" customHeight="1"/>
-    <row r="284" ht="15.75" customHeight="1"/>
-    <row r="285" ht="15.75" customHeight="1"/>
-    <row r="286" ht="15.75" customHeight="1"/>
-    <row r="287" ht="15.75" customHeight="1"/>
-    <row r="288" ht="15.75" customHeight="1"/>
-    <row r="289" ht="15.75" customHeight="1"/>
-    <row r="290" ht="15.75" customHeight="1"/>
-    <row r="291" ht="15.75" customHeight="1"/>
-    <row r="292" ht="15.75" customHeight="1"/>
-    <row r="293" ht="15.75" customHeight="1"/>
-    <row r="294" ht="15.75" customHeight="1"/>
-    <row r="295" ht="15.75" customHeight="1"/>
-    <row r="296" ht="15.75" customHeight="1"/>
-    <row r="297" ht="15.75" customHeight="1"/>
-    <row r="298" ht="15.75" customHeight="1"/>
-    <row r="299" ht="15.75" customHeight="1"/>
-    <row r="300" ht="15.75" customHeight="1"/>
-    <row r="301" ht="15.75" customHeight="1"/>
-    <row r="302" ht="15.75" customHeight="1"/>
-    <row r="303" ht="15.75" customHeight="1"/>
-    <row r="304" ht="15.75" customHeight="1"/>
-    <row r="305" ht="15.75" customHeight="1"/>
-    <row r="306" ht="15.75" customHeight="1"/>
-    <row r="307" ht="15.75" customHeight="1"/>
-    <row r="308" ht="15.75" customHeight="1"/>
-    <row r="309" ht="15.75" customHeight="1"/>
-    <row r="310" ht="15.75" customHeight="1"/>
-    <row r="311" ht="15.75" customHeight="1"/>
-    <row r="312" ht="15.75" customHeight="1"/>
-    <row r="313" ht="15.75" customHeight="1"/>
-    <row r="314" ht="15.75" customHeight="1"/>
-    <row r="315" ht="15.75" customHeight="1"/>
-    <row r="316" ht="15.75" customHeight="1"/>
-    <row r="317" ht="15.75" customHeight="1"/>
-    <row r="318" ht="15.75" customHeight="1"/>
-    <row r="319" ht="15.75" customHeight="1"/>
-    <row r="320" ht="15.75" customHeight="1"/>
-    <row r="321" ht="15.75" customHeight="1"/>
-    <row r="322" ht="15.75" customHeight="1"/>
-    <row r="323" ht="15.75" customHeight="1"/>
-    <row r="324" ht="15.75" customHeight="1"/>
-    <row r="325" ht="15.75" customHeight="1"/>
-    <row r="326" ht="15.75" customHeight="1"/>
-    <row r="327" ht="15.75" customHeight="1"/>
-    <row r="328" ht="15.75" customHeight="1"/>
-    <row r="329" ht="15.75" customHeight="1"/>
-    <row r="330" ht="15.75" customHeight="1"/>
-    <row r="331" ht="15.75" customHeight="1"/>
-    <row r="332" ht="15.75" customHeight="1"/>
-    <row r="333" ht="15.75" customHeight="1"/>
-    <row r="334" ht="15.75" customHeight="1"/>
-    <row r="335" ht="15.75" customHeight="1"/>
-    <row r="336" ht="15.75" customHeight="1"/>
-    <row r="337" ht="15.75" customHeight="1"/>
-    <row r="338" ht="15.75" customHeight="1"/>
-    <row r="339" ht="15.75" customHeight="1"/>
-    <row r="340" ht="15.75" customHeight="1"/>
-    <row r="341" ht="15.75" customHeight="1"/>
-    <row r="342" ht="15.75" customHeight="1"/>
-    <row r="343" ht="15.75" customHeight="1"/>
-    <row r="344" ht="15.75" customHeight="1"/>
-    <row r="345" ht="15.75" customHeight="1"/>
-    <row r="346" ht="15.75" customHeight="1"/>
-    <row r="347" ht="15.75" customHeight="1"/>
-    <row r="348" ht="15.75" customHeight="1"/>
-    <row r="349" ht="15.75" customHeight="1"/>
-    <row r="350" ht="15.75" customHeight="1"/>
-    <row r="351" ht="15.75" customHeight="1"/>
-    <row r="352" ht="15.75" customHeight="1"/>
-    <row r="353" ht="15.75" customHeight="1"/>
-    <row r="354" ht="15.75" customHeight="1"/>
-    <row r="355" ht="15.75" customHeight="1"/>
-    <row r="356" ht="15.75" customHeight="1"/>
-    <row r="357" ht="15.75" customHeight="1"/>
-    <row r="358" ht="15.75" customHeight="1"/>
-    <row r="359" ht="15.75" customHeight="1"/>
-    <row r="360" ht="15.75" customHeight="1"/>
-    <row r="361" ht="15.75" customHeight="1"/>
-    <row r="362" ht="15.75" customHeight="1"/>
-    <row r="363" ht="15.75" customHeight="1"/>
-    <row r="364" ht="15.75" customHeight="1"/>
-    <row r="365" ht="15.75" customHeight="1"/>
-    <row r="366" ht="15.75" customHeight="1"/>
-    <row r="367" ht="15.75" customHeight="1"/>
-    <row r="368" ht="15.75" customHeight="1"/>
-    <row r="369" ht="15.75" customHeight="1"/>
-    <row r="370" ht="15.75" customHeight="1"/>
-    <row r="371" ht="15.75" customHeight="1"/>
-    <row r="372" ht="15.75" customHeight="1"/>
-    <row r="373" ht="15.75" customHeight="1"/>
-    <row r="374" ht="15.75" customHeight="1"/>
-    <row r="375" ht="15.75" customHeight="1"/>
-    <row r="376" ht="15.75" customHeight="1"/>
-    <row r="377" ht="15.75" customHeight="1"/>
-    <row r="378" ht="15.75" customHeight="1"/>
-    <row r="379" ht="15.75" customHeight="1"/>
-    <row r="380" ht="15.75" customHeight="1"/>
-    <row r="381" ht="15.75" customHeight="1"/>
-    <row r="382" ht="15.75" customHeight="1"/>
-    <row r="383" ht="15.75" customHeight="1"/>
-    <row r="384" ht="15.75" customHeight="1"/>
-    <row r="385" ht="15.75" customHeight="1"/>
-    <row r="386" ht="15.75" customHeight="1"/>
-    <row r="387" ht="15.75" customHeight="1"/>
-    <row r="388" ht="15.75" customHeight="1"/>
-    <row r="389" ht="15.75" customHeight="1"/>
-    <row r="390" ht="15.75" customHeight="1"/>
-    <row r="391" ht="15.75" customHeight="1"/>
-    <row r="392" ht="15.75" customHeight="1"/>
-    <row r="393" ht="15.75" customHeight="1"/>
-    <row r="394" ht="15.75" customHeight="1"/>
-    <row r="395" ht="15.75" customHeight="1"/>
-    <row r="396" ht="15.75" customHeight="1"/>
-    <row r="397" ht="15.75" customHeight="1"/>
-    <row r="398" ht="15.75" customHeight="1"/>
-    <row r="399" ht="15.75" customHeight="1"/>
-    <row r="400" ht="15.75" customHeight="1"/>
-    <row r="401" ht="15.75" customHeight="1"/>
-    <row r="402" ht="15.75" customHeight="1"/>
-    <row r="403" ht="15.75" customHeight="1"/>
-    <row r="404" ht="15.75" customHeight="1"/>
-    <row r="405" ht="15.75" customHeight="1"/>
-    <row r="406" ht="15.75" customHeight="1"/>
-    <row r="407" ht="15.75" customHeight="1"/>
-    <row r="408" ht="15.75" customHeight="1"/>
-    <row r="409" ht="15.75" customHeight="1"/>
-    <row r="410" ht="15.75" customHeight="1"/>
-    <row r="411" ht="15.75" customHeight="1"/>
-    <row r="412" ht="15.75" customHeight="1"/>
-    <row r="413" ht="15.75" customHeight="1"/>
-    <row r="414" ht="15.75" customHeight="1"/>
-    <row r="415" ht="15.75" customHeight="1"/>
-    <row r="416" ht="15.75" customHeight="1"/>
-    <row r="417" ht="15.75" customHeight="1"/>
-    <row r="418" ht="15.75" customHeight="1"/>
-    <row r="419" ht="15.75" customHeight="1"/>
-    <row r="420" ht="15.75" customHeight="1"/>
-    <row r="421" ht="15.75" customHeight="1"/>
-    <row r="422" ht="15.75" customHeight="1"/>
-    <row r="423" ht="15.75" customHeight="1"/>
-    <row r="424" ht="15.75" customHeight="1"/>
-    <row r="425" ht="15.75" customHeight="1"/>
-    <row r="426" ht="15.75" customHeight="1"/>
-    <row r="427" ht="15.75" customHeight="1"/>
-    <row r="428" ht="15.75" customHeight="1"/>
-    <row r="429" ht="15.75" customHeight="1"/>
-    <row r="430" ht="15.75" customHeight="1"/>
-    <row r="431" ht="15.75" customHeight="1"/>
-    <row r="432" ht="15.75" customHeight="1"/>
-    <row r="433" ht="15.75" customHeight="1"/>
-    <row r="434" ht="15.75" customHeight="1"/>
-    <row r="435" ht="15.75" customHeight="1"/>
-    <row r="436" ht="15.75" customHeight="1"/>
-    <row r="437" ht="15.75" customHeight="1"/>
-    <row r="438" ht="15.75" customHeight="1"/>
-    <row r="439" ht="15.75" customHeight="1"/>
-    <row r="440" ht="15.75" customHeight="1"/>
-    <row r="441" ht="15.75" customHeight="1"/>
-    <row r="442" ht="15.75" customHeight="1"/>
-    <row r="443" ht="15.75" customHeight="1"/>
-    <row r="444" ht="15.75" customHeight="1"/>
-    <row r="445" ht="15.75" customHeight="1"/>
-    <row r="446" ht="15.75" customHeight="1"/>
-    <row r="447" ht="15.75" customHeight="1"/>
-    <row r="448" ht="15.75" customHeight="1"/>
-    <row r="449" ht="15.75" customHeight="1"/>
-    <row r="450" ht="15.75" customHeight="1"/>
-    <row r="451" ht="15.75" customHeight="1"/>
-    <row r="452" ht="15.75" customHeight="1"/>
-    <row r="453" ht="15.75" customHeight="1"/>
-    <row r="454" ht="15.75" customHeight="1"/>
-    <row r="455" ht="15.75" customHeight="1"/>
-    <row r="456" ht="15.75" customHeight="1"/>
-    <row r="457" ht="15.75" customHeight="1"/>
-    <row r="458" ht="15.75" customHeight="1"/>
-    <row r="459" ht="15.75" customHeight="1"/>
-    <row r="460" ht="15.75" customHeight="1"/>
-    <row r="461" ht="15.75" customHeight="1"/>
-    <row r="462" ht="15.75" customHeight="1"/>
-    <row r="463" ht="15.75" customHeight="1"/>
-    <row r="464" ht="15.75" customHeight="1"/>
-    <row r="465" ht="15.75" customHeight="1"/>
-    <row r="466" ht="15.75" customHeight="1"/>
-    <row r="467" ht="15.75" customHeight="1"/>
-    <row r="468" ht="15.75" customHeight="1"/>
-    <row r="469" ht="15.75" customHeight="1"/>
-    <row r="470" ht="15.75" customHeight="1"/>
-    <row r="471" ht="15.75" customHeight="1"/>
-    <row r="472" ht="15.75" customHeight="1"/>
-    <row r="473" ht="15.75" customHeight="1"/>
-    <row r="474" ht="15.75" customHeight="1"/>
-    <row r="475" ht="15.75" customHeight="1"/>
-    <row r="476" ht="15.75" customHeight="1"/>
-    <row r="477" ht="15.75" customHeight="1"/>
-    <row r="478" ht="15.75" customHeight="1"/>
-    <row r="479" ht="15.75" customHeight="1"/>
-    <row r="480" ht="15.75" customHeight="1"/>
-    <row r="481" ht="15.75" customHeight="1"/>
-    <row r="482" ht="15.75" customHeight="1"/>
-    <row r="483" ht="15.75" customHeight="1"/>
-    <row r="484" ht="15.75" customHeight="1"/>
-    <row r="485" ht="15.75" customHeight="1"/>
-    <row r="486" ht="15.75" customHeight="1"/>
-    <row r="487" ht="15.75" customHeight="1"/>
-    <row r="488" ht="15.75" customHeight="1"/>
-    <row r="489" ht="15.75" customHeight="1"/>
-    <row r="490" ht="15.75" customHeight="1"/>
-    <row r="491" ht="15.75" customHeight="1"/>
-    <row r="492" ht="15.75" customHeight="1"/>
-    <row r="493" ht="15.75" customHeight="1"/>
-    <row r="494" ht="15.75" customHeight="1"/>
-    <row r="495" ht="15.75" customHeight="1"/>
-    <row r="496" ht="15.75" customHeight="1"/>
-    <row r="497" ht="15.75" customHeight="1"/>
-    <row r="498" ht="15.75" customHeight="1"/>
-    <row r="499" ht="15.75" customHeight="1"/>
-    <row r="500" ht="15.75" customHeight="1"/>
-    <row r="501" ht="15.75" customHeight="1"/>
-    <row r="502" ht="15.75" customHeight="1"/>
-    <row r="503" ht="15.75" customHeight="1"/>
-    <row r="504" ht="15.75" customHeight="1"/>
-    <row r="505" ht="15.75" customHeight="1"/>
-    <row r="506" ht="15.75" customHeight="1"/>
-    <row r="507" ht="15.75" customHeight="1"/>
-    <row r="508" ht="15.75" customHeight="1"/>
-    <row r="509" ht="15.75" customHeight="1"/>
-    <row r="510" ht="15.75" customHeight="1"/>
-    <row r="511" ht="15.75" customHeight="1"/>
-    <row r="512" ht="15.75" customHeight="1"/>
-    <row r="513" ht="15.75" customHeight="1"/>
-    <row r="514" ht="15.75" customHeight="1"/>
-    <row r="515" ht="15.75" customHeight="1"/>
-    <row r="516" ht="15.75" customHeight="1"/>
-    <row r="517" ht="15.75" customHeight="1"/>
-    <row r="518" ht="15.75" customHeight="1"/>
-    <row r="519" ht="15.75" customHeight="1"/>
-    <row r="520" ht="15.75" customHeight="1"/>
-    <row r="521" ht="15.75" customHeight="1"/>
-    <row r="522" ht="15.75" customHeight="1"/>
-    <row r="523" ht="15.75" customHeight="1"/>
-    <row r="524" ht="15.75" customHeight="1"/>
-    <row r="525" ht="15.75" customHeight="1"/>
-    <row r="526" ht="15.75" customHeight="1"/>
-    <row r="527" ht="15.75" customHeight="1"/>
-    <row r="528" ht="15.75" customHeight="1"/>
-    <row r="529" ht="15.75" customHeight="1"/>
-    <row r="530" ht="15.75" customHeight="1"/>
-    <row r="531" ht="15.75" customHeight="1"/>
-    <row r="532" ht="15.75" customHeight="1"/>
-    <row r="533" ht="15.75" customHeight="1"/>
-    <row r="534" ht="15.75" customHeight="1"/>
-    <row r="535" ht="15.75" customHeight="1"/>
-    <row r="536" ht="15.75" customHeight="1"/>
-    <row r="537" ht="15.75" customHeight="1"/>
-    <row r="538" ht="15.75" customHeight="1"/>
-    <row r="539" ht="15.75" customHeight="1"/>
-    <row r="540" ht="15.75" customHeight="1"/>
-    <row r="541" ht="15.75" customHeight="1"/>
-    <row r="542" ht="15.75" customHeight="1"/>
-    <row r="543" ht="15.75" customHeight="1"/>
-    <row r="544" ht="15.75" customHeight="1"/>
-    <row r="545" ht="15.75" customHeight="1"/>
-    <row r="546" ht="15.75" customHeight="1"/>
-    <row r="547" ht="15.75" customHeight="1"/>
-    <row r="548" ht="15.75" customHeight="1"/>
-    <row r="549" ht="15.75" customHeight="1"/>
-    <row r="550" ht="15.75" customHeight="1"/>
-    <row r="551" ht="15.75" customHeight="1"/>
-    <row r="552" ht="15.75" customHeight="1"/>
-    <row r="553" ht="15.75" customHeight="1"/>
-    <row r="554" ht="15.75" customHeight="1"/>
-    <row r="555" ht="15.75" customHeight="1"/>
-    <row r="556" ht="15.75" customHeight="1"/>
-    <row r="557" ht="15.75" customHeight="1"/>
-    <row r="558" ht="15.75" customHeight="1"/>
-    <row r="559" ht="15.75" customHeight="1"/>
-    <row r="560" ht="15.75" customHeight="1"/>
-    <row r="561" ht="15.75" customHeight="1"/>
-    <row r="562" ht="15.75" customHeight="1"/>
-    <row r="563" ht="15.75" customHeight="1"/>
-    <row r="564" ht="15.75" customHeight="1"/>
-    <row r="565" ht="15.75" customHeight="1"/>
-    <row r="566" ht="15.75" customHeight="1"/>
-    <row r="567" ht="15.75" customHeight="1"/>
-    <row r="568" ht="15.75" customHeight="1"/>
-    <row r="569" ht="15.75" customHeight="1"/>
-    <row r="570" ht="15.75" customHeight="1"/>
-    <row r="571" ht="15.75" customHeight="1"/>
-    <row r="572" ht="15.75" customHeight="1"/>
-    <row r="573" ht="15.75" customHeight="1"/>
-    <row r="574" ht="15.75" customHeight="1"/>
-    <row r="575" ht="15.75" customHeight="1"/>
-    <row r="576" ht="15.75" customHeight="1"/>
-    <row r="577" ht="15.75" customHeight="1"/>
-    <row r="578" ht="15.75" customHeight="1"/>
-    <row r="579" ht="15.75" customHeight="1"/>
-    <row r="580" ht="15.75" customHeight="1"/>
-    <row r="581" ht="15.75" customHeight="1"/>
-    <row r="582" ht="15.75" customHeight="1"/>
-    <row r="583" ht="15.75" customHeight="1"/>
-    <row r="584" ht="15.75" customHeight="1"/>
-    <row r="585" ht="15.75" customHeight="1"/>
-    <row r="586" ht="15.75" customHeight="1"/>
-    <row r="587" ht="15.75" customHeight="1"/>
-    <row r="588" ht="15.75" customHeight="1"/>
-    <row r="589" ht="15.75" customHeight="1"/>
-    <row r="590" ht="15.75" customHeight="1"/>
-    <row r="591" ht="15.75" customHeight="1"/>
-    <row r="592" ht="15.75" customHeight="1"/>
-    <row r="593" ht="15.75" customHeight="1"/>
-    <row r="594" ht="15.75" customHeight="1"/>
-    <row r="595" ht="15.75" customHeight="1"/>
-    <row r="596" ht="15.75" customHeight="1"/>
-    <row r="597" ht="15.75" customHeight="1"/>
-    <row r="598" ht="15.75" customHeight="1"/>
-    <row r="599" ht="15.75" customHeight="1"/>
-    <row r="600" ht="15.75" customHeight="1"/>
-    <row r="601" ht="15.75" customHeight="1"/>
-    <row r="602" ht="15.75" customHeight="1"/>
-    <row r="603" ht="15.75" customHeight="1"/>
-    <row r="604" ht="15.75" customHeight="1"/>
-    <row r="605" ht="15.75" customHeight="1"/>
-    <row r="606" ht="15.75" customHeight="1"/>
-    <row r="607" ht="15.75" customHeight="1"/>
-    <row r="608" ht="15.75" customHeight="1"/>
-    <row r="609" ht="15.75" customHeight="1"/>
-    <row r="610" ht="15.75" customHeight="1"/>
-    <row r="611" ht="15.75" customHeight="1"/>
-    <row r="612" ht="15.75" customHeight="1"/>
-    <row r="613" ht="15.75" customHeight="1"/>
-    <row r="614" ht="15.75" customHeight="1"/>
-    <row r="615" ht="15.75" customHeight="1"/>
-    <row r="616" ht="15.75" customHeight="1"/>
-    <row r="617" ht="15.75" customHeight="1"/>
-    <row r="618" ht="15.75" customHeight="1"/>
-    <row r="619" ht="15.75" customHeight="1"/>
-    <row r="620" ht="15.75" customHeight="1"/>
-    <row r="621" ht="15.75" customHeight="1"/>
-    <row r="622" ht="15.75" customHeight="1"/>
-    <row r="623" ht="15.75" customHeight="1"/>
-    <row r="624" ht="15.75" customHeight="1"/>
-    <row r="625" ht="15.75" customHeight="1"/>
-    <row r="626" ht="15.75" customHeight="1"/>
-    <row r="627" ht="15.75" customHeight="1"/>
-    <row r="628" ht="15.75" customHeight="1"/>
-    <row r="629" ht="15.75" customHeight="1"/>
-    <row r="630" ht="15.75" customHeight="1"/>
-    <row r="631" ht="15.75" customHeight="1"/>
-    <row r="632" ht="15.75" customHeight="1"/>
-    <row r="633" ht="15.75" customHeight="1"/>
-    <row r="634" ht="15.75" customHeight="1"/>
-    <row r="635" ht="15.75" customHeight="1"/>
-    <row r="636" ht="15.75" customHeight="1"/>
-    <row r="637" ht="15.75" customHeight="1"/>
-    <row r="638" ht="15.75" customHeight="1"/>
-    <row r="639" ht="15.75" customHeight="1"/>
-    <row r="640" ht="15.75" customHeight="1"/>
-    <row r="641" ht="15.75" customHeight="1"/>
-    <row r="642" ht="15.75" customHeight="1"/>
-    <row r="643" ht="15.75" customHeight="1"/>
-    <row r="644" ht="15.75" customHeight="1"/>
-    <row r="645" ht="15.75" customHeight="1"/>
-    <row r="646" ht="15.75" customHeight="1"/>
-    <row r="647" ht="15.75" customHeight="1"/>
-    <row r="648" ht="15.75" customHeight="1"/>
-    <row r="649" ht="15.75" customHeight="1"/>
-    <row r="650" ht="15.75" customHeight="1"/>
-    <row r="651" ht="15.75" customHeight="1"/>
-    <row r="652" ht="15.75" customHeight="1"/>
-    <row r="653" ht="15.75" customHeight="1"/>
-    <row r="654" ht="15.75" customHeight="1"/>
-    <row r="655" ht="15.75" customHeight="1"/>
-    <row r="656" ht="15.75" customHeight="1"/>
-    <row r="657" ht="15.75" customHeight="1"/>
-    <row r="658" ht="15.75" customHeight="1"/>
-    <row r="659" ht="15.75" customHeight="1"/>
-    <row r="660" ht="15.75" customHeight="1"/>
-    <row r="661" ht="15.75" customHeight="1"/>
-    <row r="662" ht="15.75" customHeight="1"/>
-    <row r="663" ht="15.75" customHeight="1"/>
-    <row r="664" ht="15.75" customHeight="1"/>
-    <row r="665" ht="15.75" customHeight="1"/>
-    <row r="666" ht="15.75" customHeight="1"/>
-    <row r="667" ht="15.75" customHeight="1"/>
-    <row r="668" ht="15.75" customHeight="1"/>
-    <row r="669" ht="15.75" customHeight="1"/>
-    <row r="670" ht="15.75" customHeight="1"/>
-    <row r="671" ht="15.75" customHeight="1"/>
-    <row r="672" ht="15.75" customHeight="1"/>
-    <row r="673" ht="15.75" customHeight="1"/>
-    <row r="674" ht="15.75" customHeight="1"/>
-    <row r="675" ht="15.75" customHeight="1"/>
-    <row r="676" ht="15.75" customHeight="1"/>
-    <row r="677" ht="15.75" customHeight="1"/>
-    <row r="678" ht="15.75" customHeight="1"/>
-    <row r="679" ht="15.75" customHeight="1"/>
-    <row r="680" ht="15.75" customHeight="1"/>
-    <row r="681" ht="15.75" customHeight="1"/>
-    <row r="682" ht="15.75" customHeight="1"/>
-    <row r="683" ht="15.75" customHeight="1"/>
-    <row r="684" ht="15.75" customHeight="1"/>
-    <row r="685" ht="15.75" customHeight="1"/>
-    <row r="686" ht="15.75" customHeight="1"/>
-    <row r="687" ht="15.75" customHeight="1"/>
-    <row r="688" ht="15.75" customHeight="1"/>
-    <row r="689" ht="15.75" customHeight="1"/>
-    <row r="690" ht="15.75" customHeight="1"/>
-    <row r="691" ht="15.75" customHeight="1"/>
-    <row r="692" ht="15.75" customHeight="1"/>
-    <row r="693" ht="15.75" customHeight="1"/>
-    <row r="694" ht="15.75" customHeight="1"/>
-    <row r="695" ht="15.75" customHeight="1"/>
-    <row r="696" ht="15.75" customHeight="1"/>
-    <row r="697" ht="15.75" customHeight="1"/>
-    <row r="698" ht="15.75" customHeight="1"/>
-    <row r="699" ht="15.75" customHeight="1"/>
-    <row r="700" ht="15.75" customHeight="1"/>
-    <row r="701" ht="15.75" customHeight="1"/>
-    <row r="702" ht="15.75" customHeight="1"/>
-    <row r="703" ht="15.75" customHeight="1"/>
-    <row r="704" ht="15.75" customHeight="1"/>
-    <row r="705" ht="15.75" customHeight="1"/>
-    <row r="706" ht="15.75" customHeight="1"/>
-    <row r="707" ht="15.75" customHeight="1"/>
-    <row r="708" ht="15.75" customHeight="1"/>
-    <row r="709" ht="15.75" customHeight="1"/>
-    <row r="710" ht="15.75" customHeight="1"/>
-    <row r="711" ht="15.75" customHeight="1"/>
-    <row r="712" ht="15.75" customHeight="1"/>
-    <row r="713" ht="15.75" customHeight="1"/>
-    <row r="714" ht="15.75" customHeight="1"/>
-    <row r="715" ht="15.75" customHeight="1"/>
-    <row r="716" ht="15.75" customHeight="1"/>
-    <row r="717" ht="15.75" customHeight="1"/>
-    <row r="718" ht="15.75" customHeight="1"/>
-    <row r="719" ht="15.75" customHeight="1"/>
-    <row r="720" ht="15.75" customHeight="1"/>
-    <row r="721" ht="15.75" customHeight="1"/>
-    <row r="722" ht="15.75" customHeight="1"/>
-    <row r="723" ht="15.75" customHeight="1"/>
-    <row r="724" ht="15.75" customHeight="1"/>
-    <row r="725" ht="15.75" customHeight="1"/>
-    <row r="726" ht="15.75" customHeight="1"/>
-    <row r="727" ht="15.75" customHeight="1"/>
-    <row r="728" ht="15.75" customHeight="1"/>
-    <row r="729" ht="15.75" customHeight="1"/>
-    <row r="730" ht="15.75" customHeight="1"/>
-    <row r="731" ht="15.75" customHeight="1"/>
-    <row r="732" ht="15.75" customHeight="1"/>
-    <row r="733" ht="15.75" customHeight="1"/>
-    <row r="734" ht="15.75" customHeight="1"/>
-    <row r="735" ht="15.75" customHeight="1"/>
-    <row r="736" ht="15.75" customHeight="1"/>
-    <row r="737" ht="15.75" customHeight="1"/>
-    <row r="738" ht="15.75" customHeight="1"/>
-    <row r="739" ht="15.75" customHeight="1"/>
-    <row r="740" ht="15.75" customHeight="1"/>
-    <row r="741" ht="15.75" customHeight="1"/>
-    <row r="742" ht="15.75" customHeight="1"/>
-    <row r="743" ht="15.75" customHeight="1"/>
-    <row r="744" ht="15.75" customHeight="1"/>
-    <row r="745" ht="15.75" customHeight="1"/>
-    <row r="746" ht="15.75" customHeight="1"/>
-    <row r="747" ht="15.75" customHeight="1"/>
-    <row r="748" ht="15.75" customHeight="1"/>
-    <row r="749" ht="15.75" customHeight="1"/>
-    <row r="750" ht="15.75" customHeight="1"/>
-    <row r="751" ht="15.75" customHeight="1"/>
-    <row r="752" ht="15.75" customHeight="1"/>
-    <row r="753" ht="15.75" customHeight="1"/>
-    <row r="754" ht="15.75" customHeight="1"/>
-    <row r="755" ht="15.75" customHeight="1"/>
-    <row r="756" ht="15.75" customHeight="1"/>
-    <row r="757" ht="15.75" customHeight="1"/>
-    <row r="758" ht="15.75" customHeight="1"/>
-    <row r="759" ht="15.75" customHeight="1"/>
-    <row r="760" ht="15.75" customHeight="1"/>
-    <row r="761" ht="15.75" customHeight="1"/>
-    <row r="762" ht="15.75" customHeight="1"/>
-    <row r="763" ht="15.75" customHeight="1"/>
-    <row r="764" ht="15.75" customHeight="1"/>
-    <row r="765" ht="15.75" customHeight="1"/>
-    <row r="766" ht="15.75" customHeight="1"/>
-    <row r="767" ht="15.75" customHeight="1"/>
-    <row r="768" ht="15.75" customHeight="1"/>
-    <row r="769" ht="15.75" customHeight="1"/>
-    <row r="770" ht="15.75" customHeight="1"/>
-    <row r="771" ht="15.75" customHeight="1"/>
-    <row r="772" ht="15.75" customHeight="1"/>
-    <row r="773" ht="15.75" customHeight="1"/>
-    <row r="774" ht="15.75" customHeight="1"/>
-    <row r="775" ht="15.75" customHeight="1"/>
-    <row r="776" ht="15.75" customHeight="1"/>
-    <row r="777" ht="15.75" customHeight="1"/>
-    <row r="778" ht="15.75" customHeight="1"/>
-    <row r="779" ht="15.75" customHeight="1"/>
-    <row r="780" ht="15.75" customHeight="1"/>
-    <row r="781" ht="15.75" customHeight="1"/>
-    <row r="782" ht="15.75" customHeight="1"/>
-    <row r="783" ht="15.75" customHeight="1"/>
-    <row r="784" ht="15.75" customHeight="1"/>
-    <row r="785" ht="15.75" customHeight="1"/>
-    <row r="786" ht="15.75" customHeight="1"/>
-    <row r="787" ht="15.75" customHeight="1"/>
-    <row r="788" ht="15.75" customHeight="1"/>
-    <row r="789" ht="15.75" customHeight="1"/>
-    <row r="790" ht="15.75" customHeight="1"/>
-    <row r="791" ht="15.75" customHeight="1"/>
-    <row r="792" ht="15.75" customHeight="1"/>
-    <row r="793" ht="15.75" customHeight="1"/>
-    <row r="794" ht="15.75" customHeight="1"/>
-    <row r="795" ht="15.75" customHeight="1"/>
-    <row r="796" ht="15.75" customHeight="1"/>
-    <row r="797" ht="15.75" customHeight="1"/>
-    <row r="798" ht="15.75" customHeight="1"/>
-    <row r="799" ht="15.75" customHeight="1"/>
-    <row r="800" ht="15.75" customHeight="1"/>
-    <row r="801" ht="15.75" customHeight="1"/>
-    <row r="802" ht="15.75" customHeight="1"/>
-    <row r="803" ht="15.75" customHeight="1"/>
-    <row r="804" ht="15.75" customHeight="1"/>
-    <row r="805" ht="15.75" customHeight="1"/>
-    <row r="806" ht="15.75" customHeight="1"/>
-    <row r="807" ht="15.75" customHeight="1"/>
-    <row r="808" ht="15.75" customHeight="1"/>
-    <row r="809" ht="15.75" customHeight="1"/>
-    <row r="810" ht="15.75" customHeight="1"/>
-    <row r="811" ht="15.75" customHeight="1"/>
-    <row r="812" ht="15.75" customHeight="1"/>
-    <row r="813" ht="15.75" customHeight="1"/>
-    <row r="814" ht="15.75" customHeight="1"/>
-    <row r="815" ht="15.75" customHeight="1"/>
-    <row r="816" ht="15.75" customHeight="1"/>
-    <row r="817" ht="15.75" customHeight="1"/>
-    <row r="818" ht="15.75" customHeight="1"/>
-    <row r="819" ht="15.75" customHeight="1"/>
-    <row r="820" ht="15.75" customHeight="1"/>
-    <row r="821" ht="15.75" customHeight="1"/>
-    <row r="822" ht="15.75" customHeight="1"/>
-    <row r="823" ht="15.75" customHeight="1"/>
-    <row r="824" ht="15.75" customHeight="1"/>
-    <row r="825" ht="15.75" customHeight="1"/>
-    <row r="826" ht="15.75" customHeight="1"/>
-    <row r="827" ht="15.75" customHeight="1"/>
-    <row r="828" ht="15.75" customHeight="1"/>
-    <row r="829" ht="15.75" customHeight="1"/>
-    <row r="830" ht="15.75" customHeight="1"/>
-    <row r="831" ht="15.75" customHeight="1"/>
-    <row r="832" ht="15.75" customHeight="1"/>
-    <row r="833" ht="15.75" customHeight="1"/>
-    <row r="834" ht="15.75" customHeight="1"/>
-    <row r="835" ht="15.75" customHeight="1"/>
-    <row r="836" ht="15.75" customHeight="1"/>
-    <row r="837" ht="15.75" customHeight="1"/>
-    <row r="838" ht="15.75" customHeight="1"/>
-    <row r="839" ht="15.75" customHeight="1"/>
-    <row r="840" ht="15.75" customHeight="1"/>
-    <row r="841" ht="15.75" customHeight="1"/>
-    <row r="842" ht="15.75" customHeight="1"/>
-    <row r="843" ht="15.75" customHeight="1"/>
-    <row r="844" ht="15.75" customHeight="1"/>
-    <row r="845" ht="15.75" customHeight="1"/>
-    <row r="846" ht="15.75" customHeight="1"/>
-    <row r="847" ht="15.75" customHeight="1"/>
-    <row r="848" ht="15.75" customHeight="1"/>
-    <row r="849" ht="15.75" customHeight="1"/>
-    <row r="850" ht="15.75" customHeight="1"/>
-    <row r="851" ht="15.75" customHeight="1"/>
-    <row r="852" ht="15.75" customHeight="1"/>
-    <row r="853" ht="15.75" customHeight="1"/>
-    <row r="854" ht="15.75" customHeight="1"/>
-    <row r="855" ht="15.75" customHeight="1"/>
-    <row r="856" ht="15.75" customHeight="1"/>
-    <row r="857" ht="15.75" customHeight="1"/>
-    <row r="858" ht="15.75" customHeight="1"/>
-    <row r="859" ht="15.75" customHeight="1"/>
-    <row r="860" ht="15.75" customHeight="1"/>
-    <row r="861" ht="15.75" customHeight="1"/>
-    <row r="862" ht="15.75" customHeight="1"/>
-    <row r="863" ht="15.75" customHeight="1"/>
-    <row r="864" ht="15.75" customHeight="1"/>
-    <row r="865" ht="15.75" customHeight="1"/>
-    <row r="866" ht="15.75" customHeight="1"/>
-    <row r="867" ht="15.75" customHeight="1"/>
-    <row r="868" ht="15.75" customHeight="1"/>
-    <row r="869" ht="15.75" customHeight="1"/>
-    <row r="870" ht="15.75" customHeight="1"/>
-    <row r="871" ht="15.75" customHeight="1"/>
-    <row r="872" ht="15.75" customHeight="1"/>
-    <row r="873" ht="15.75" customHeight="1"/>
-    <row r="874" ht="15.75" customHeight="1"/>
-    <row r="875" ht="15.75" customHeight="1"/>
-    <row r="876" ht="15.75" customHeight="1"/>
-    <row r="877" ht="15.75" customHeight="1"/>
-    <row r="878" ht="15.75" customHeight="1"/>
-    <row r="879" ht="15.75" customHeight="1"/>
-    <row r="880" ht="15.75" customHeight="1"/>
-    <row r="881" ht="15.75" customHeight="1"/>
-    <row r="882" ht="15.75" customHeight="1"/>
-    <row r="883" ht="15.75" customHeight="1"/>
-    <row r="884" ht="15.75" customHeight="1"/>
-    <row r="885" ht="15.75" customHeight="1"/>
-    <row r="886" ht="15.75" customHeight="1"/>
-    <row r="887" ht="15.75" customHeight="1"/>
-    <row r="888" ht="15.75" customHeight="1"/>
-    <row r="889" ht="15.75" customHeight="1"/>
-    <row r="890" ht="15.75" customHeight="1"/>
-    <row r="891" ht="15.75" customHeight="1"/>
-    <row r="892" ht="15.75" customHeight="1"/>
-    <row r="893" ht="15.75" customHeight="1"/>
-    <row r="894" ht="15.75" customHeight="1"/>
-    <row r="895" ht="15.75" customHeight="1"/>
-    <row r="896" ht="15.75" customHeight="1"/>
-    <row r="897" ht="15.75" customHeight="1"/>
-    <row r="898" ht="15.75" customHeight="1"/>
-    <row r="899" ht="15.75" customHeight="1"/>
-    <row r="900" ht="15.75" customHeight="1"/>
-    <row r="901" ht="15.75" customHeight="1"/>
-    <row r="902" ht="15.75" customHeight="1"/>
-    <row r="903" ht="15.75" customHeight="1"/>
-    <row r="904" ht="15.75" customHeight="1"/>
-    <row r="905" ht="15.75" customHeight="1"/>
-    <row r="906" ht="15.75" customHeight="1"/>
-    <row r="907" ht="15.75" customHeight="1"/>
-    <row r="908" ht="15.75" customHeight="1"/>
-    <row r="909" ht="15.75" customHeight="1"/>
-    <row r="910" ht="15.75" customHeight="1"/>
-    <row r="911" ht="15.75" customHeight="1"/>
-    <row r="912" ht="15.75" customHeight="1"/>
-    <row r="913" ht="15.75" customHeight="1"/>
-    <row r="914" ht="15.75" customHeight="1"/>
-    <row r="915" ht="15.75" customHeight="1"/>
-    <row r="916" ht="15.75" customHeight="1"/>
-    <row r="917" ht="15.75" customHeight="1"/>
-    <row r="918" ht="15.75" customHeight="1"/>
-    <row r="919" ht="15.75" customHeight="1"/>
-    <row r="920" ht="15.75" customHeight="1"/>
-    <row r="921" ht="15.75" customHeight="1"/>
-    <row r="922" ht="15.75" customHeight="1"/>
-    <row r="923" ht="15.75" customHeight="1"/>
-    <row r="924" ht="15.75" customHeight="1"/>
-    <row r="925" ht="15.75" customHeight="1"/>
-    <row r="926" ht="15.75" customHeight="1"/>
-    <row r="927" ht="15.75" customHeight="1"/>
-    <row r="928" ht="15.75" customHeight="1"/>
-    <row r="929" ht="15.75" customHeight="1"/>
-    <row r="930" ht="15.75" customHeight="1"/>
-    <row r="931" ht="15.75" customHeight="1"/>
-    <row r="932" ht="15.75" customHeight="1"/>
-    <row r="933" ht="15.75" customHeight="1"/>
-    <row r="934" ht="15.75" customHeight="1"/>
-    <row r="935" ht="15.75" customHeight="1"/>
-    <row r="936" ht="15.75" customHeight="1"/>
-    <row r="937" ht="15.75" customHeight="1"/>
-    <row r="938" ht="15.75" customHeight="1"/>
-    <row r="939" ht="15.75" customHeight="1"/>
-    <row r="940" ht="15.75" customHeight="1"/>
-    <row r="941" ht="15.75" customHeight="1"/>
-    <row r="942" ht="15.75" customHeight="1"/>
-    <row r="943" ht="15.75" customHeight="1"/>
-    <row r="944" ht="15.75" customHeight="1"/>
-    <row r="945" ht="15.75" customHeight="1"/>
-    <row r="946" ht="15.75" customHeight="1"/>
-    <row r="947" ht="15.75" customHeight="1"/>
-    <row r="948" ht="15.75" customHeight="1"/>
-    <row r="949" ht="15.75" customHeight="1"/>
-    <row r="950" ht="15.75" customHeight="1"/>
-    <row r="951" ht="15.75" customHeight="1"/>
-    <row r="952" ht="15.75" customHeight="1"/>
-    <row r="953" ht="15.75" customHeight="1"/>
-    <row r="954" ht="15.75" customHeight="1"/>
-    <row r="955" ht="15.75" customHeight="1"/>
-    <row r="956" ht="15.75" customHeight="1"/>
-    <row r="957" ht="15.75" customHeight="1"/>
-    <row r="958" ht="15.75" customHeight="1"/>
-    <row r="959" ht="15.75" customHeight="1"/>
-    <row r="960" ht="15.75" customHeight="1"/>
-    <row r="961" ht="15.75" customHeight="1"/>
-    <row r="962" ht="15.75" customHeight="1"/>
-    <row r="963" ht="15.75" customHeight="1"/>
-    <row r="964" ht="15.75" customHeight="1"/>
-    <row r="965" ht="15.75" customHeight="1"/>
-    <row r="966" ht="15.75" customHeight="1"/>
-    <row r="967" ht="15.75" customHeight="1"/>
-    <row r="968" ht="15.75" customHeight="1"/>
-    <row r="969" ht="15.75" customHeight="1"/>
-    <row r="970" ht="15.75" customHeight="1"/>
-    <row r="971" ht="15.75" customHeight="1"/>
-    <row r="972" ht="15.75" customHeight="1"/>
-    <row r="973" ht="15.75" customHeight="1"/>
-    <row r="974" ht="15.75" customHeight="1"/>
-    <row r="975" ht="15.75" customHeight="1"/>
-    <row r="976" ht="15.75" customHeight="1"/>
-    <row r="977" ht="15.75" customHeight="1"/>
-    <row r="978" ht="15.75" customHeight="1"/>
-    <row r="979" ht="15.75" customHeight="1"/>
-    <row r="980" ht="15.75" customHeight="1"/>
-    <row r="981" ht="15.75" customHeight="1"/>
-    <row r="982" ht="15.75" customHeight="1"/>
-    <row r="983" ht="15.75" customHeight="1"/>
-    <row r="984" ht="15.75" customHeight="1"/>
-    <row r="985" ht="15.75" customHeight="1"/>
-    <row r="986" ht="15.75" customHeight="1"/>
-    <row r="987" ht="15.75" customHeight="1"/>
-    <row r="988" ht="15.75" customHeight="1"/>
-    <row r="989" ht="15.75" customHeight="1"/>
-    <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="238" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A3:B3"/>
@@ -7936,27 +8247,56 @@
     <mergeCell ref="A25:A27"/>
     <mergeCell ref="A17:B17"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="1.05277777777778" footer="0.0" header="0.0" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1121232432</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>3243243</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>